<commit_message>
Info completa maquina 1
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4 - Maquina1.xlsx
+++ b/Docs/Tablas Lab 4 - Maquina1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Tareas\ESTRUC. DE DATOS Y ALGORITMOS\lab4\LabSorts-S04-G09\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DE72F0-AB3C-41BF-9B4B-BA38B5B3DB9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE122718-BA9F-4BD7-AB0D-9CCDA1E0978B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -588,6 +588,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.60105095202048564"/>
+                  <c:y val="0.13324571234796431"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -739,11 +745,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.60984794478813387"/>
+                  <c:y val="0.22607882742336621"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -895,10 +906,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.7080073760821777E-3"/>
+                  <c:y val="-3.2211597211065666E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1145,6 +1162,7 @@
         <c:axId val="1833162896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1314,9 +1332,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -1417,7 +1433,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10820912968533665"/>
+          <c:y val="0.10085518653783172"/>
+          <c:w val="0.85079688401742271"/>
+          <c:h val="0.74848566179666243"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -1615,11 +1641,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.60397843420686392"/>
+                  <c:y val="7.2702376429223961E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1741,10 +1772,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.2004945480002372E-3"/>
+                  <c:y val="0.67208140202475353"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1976,6 +2013,8 @@
         <c:axId val="1833162896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2300,11 +2339,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.60398328294303505"/>
+                  <c:y val="0.3146437167696936"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2456,11 +2500,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.63805696826305913"/>
+                  <c:y val="0.16126726577555139"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2692,6 +2741,8 @@
         <c:axId val="1328121328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3006,11 +3057,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.60105095202048564"/>
+                  <c:y val="0.22786493528616575"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3162,11 +3218,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.60433516265374099"/>
+                  <c:y val="0.14310426499992929"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3398,6 +3459,7 @@
         <c:axId val="1328121328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3712,8 +3774,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -3874,11 +3935,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.57356191296155057"/>
+                  <c:y val="0.14927480640459126"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4110,6 +4176,7 @@
         <c:axId val="1328121328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7123,7 +7190,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7620,8 +7687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7888,6 +7955,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="04b510ef1bc187d79b842c792d256c41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9049981c3eb1ee76226ec9e2f8ecd7b4" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -8098,15 +8174,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -8114,6 +8181,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03EB27C0-F9F6-4037-B95E-326B818673EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8132,14 +8207,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>

</xml_diff>